<commit_message>
smoke Test Cases in process; E2E Test corrected: the example of the Glossary need to rewrite screens
</commit_message>
<xml_diff>
--- a/DesignDocs/Example_Glossary_Random4Dinner.xlsx
+++ b/DesignDocs/Example_Glossary_Random4Dinner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EnyFood\Random4Dinner\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EB3811-5497-4729-8645-DDEF3E90CC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D243FA1D-F3FD-42F1-92AF-533F5D09EB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44100" yWindow="795" windowWidth="36525" windowHeight="12330" xr2:uid="{8C7EFB95-537E-4066-989B-733ADEACC89B}"/>
+    <workbookView xWindow="-51495" yWindow="465" windowWidth="27765" windowHeight="18810" xr2:uid="{8C7EFB95-537E-4066-989B-733ADEACC89B}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
@@ -61,16 +61,6 @@
     <t>"New dish" screen</t>
   </si>
   <si>
-    <t>1. "Новое блюдо" screen
-2. Back button 
-3. [Сохранить] button
-4. "{Name}" dish field
-5. Content info field
-6. Segment control
-7. Selected segment
-8. [Выбрать фото] button</t>
-  </si>
-  <si>
     <t>"Settings" screen</t>
   </si>
   <si>
@@ -159,14 +149,24 @@
 4. Back button</t>
   </si>
   <si>
+    <t>1. "Новое блюдо" screen
+2. Back button 
+3. [Сохранить] button
+4. "Name dish" field
+5. "Content info" field
+6. Segment control
+7. Selected segment
+8. [Выбрать фото] button</t>
+  </si>
+  <si>
     <t>1. [Отмена] button 
 2. [Добавить] button 
-3. "{Name} receipt field
+3. "Name" receipt field
 4. Category Picker
-5. Contetn info field
-6. Link field
+5. "Contetn info" field
+6. "Link" field
 7. Stepper
-8. Ingredients field
+8. "Ingredients" field
 9. Proportions stepper</t>
   </si>
 </sst>
@@ -293,9 +293,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -303,6 +300,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1269,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3B538B-1E03-4212-A4DA-A3DBB822E499}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1297,22 +1297,22 @@
       <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:13" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="8"/>
+      <c r="A2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="327.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:13" ht="328.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
@@ -1321,83 +1321,83 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:13" ht="342" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="339" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9" t="s">
+      <c r="A10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="365.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>24</v>
@@ -1405,6 +1405,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="I10:J10"/>
@@ -1412,11 +1417,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>